<commit_message>
Fixed up first git command so it's easier to manipulate the delimters
</commit_message>
<xml_diff>
--- a/Jan_2008_Sample.xlsx
+++ b/Jan_2008_Sample.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jan 2008 (Sample)" sheetId="2" r:id="rId1"/>
     <sheet name="RAW DATA" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Jan_2008_test_1" localSheetId="1">'RAW DATA'!$A$1:$C$47</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -133,8 +137,22 @@
 </comments>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Jan_2008_test" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\User\Documents\seng403_New\Jan_2008_test.txt" tab="0" space="1" comma="1" consecutive="1" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t xml:space="preserve">Contributor Name </t>
   </si>
@@ -176,6 +194,84 @@
   </si>
   <si>
     <t>GHTorrentName</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>a518f23a2b8b2a4499113b20057c76824ed5d1ac</t>
+  </si>
+  <si>
+    <t>db/</t>
+  </si>
+  <si>
+    <t>eef739da55fbab471e5adc76c1c7d5af0409499c</t>
+  </si>
+  <si>
+    <t>util/</t>
+  </si>
+  <si>
+    <t>9e1d56bdd0c45deede6f1aeddfe40ee7817b50cb</t>
+  </si>
+  <si>
+    <t>5795cee2f7b12d5da89f0ec565409dbaed30a5af</t>
+  </si>
+  <si>
+    <t>a3d1609506773c9c67cc2950371dd149d7f0ca4b</t>
+  </si>
+  <si>
+    <t>b9c78504dbd7d05cf93b02f2bd28d3176184e35e</t>
+  </si>
+  <si>
+    <t>e20c9d2b0df280bf3742af2b5b671a008c108436</t>
+  </si>
+  <si>
+    <t>da8ecf472130fa901330d34e38270d0e84779170</t>
+  </si>
+  <si>
+    <t>a186665dd792aabe3f2cba60880e2d8f1b5017fb</t>
+  </si>
+  <si>
+    <t>Eliot</t>
+  </si>
+  <si>
+    <t>Horowitz</t>
+  </si>
+  <si>
+    <t>093b76717eacaac4f51ec00ca67df911d8c64210</t>
+  </si>
+  <si>
+    <t>9f35516beb3b2df345022a9e97b163d7934ac635</t>
+  </si>
+  <si>
+    <t>grid/</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>573b11ecd4c9592f4199f9c6f416a372e540765e</t>
+  </si>
+  <si>
+    <t>bin/</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Commit_ShaField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total LOC </t>
+  </si>
+  <si>
+    <t>COMMIT HASHES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC </t>
   </si>
 </sst>
 </file>
@@ -230,9 +326,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,6 +345,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_test_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4545,12 +4646,334 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="13" max="13" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>0.107</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N51" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing up templates for later months
</commit_message>
<xml_diff>
--- a/Jan_2008_Sample.xlsx
+++ b/Jan_2008_Sample.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
   <si>
     <t xml:space="preserve">Contributor Name </t>
   </si>
@@ -221,9 +221,6 @@
   </si>
   <si>
     <t>Minor Components</t>
-  </si>
-  <si>
-    <t>GHTorrentName</t>
   </si>
   <si>
     <t>Dwight</t>
@@ -308,6 +305,21 @@
   </si>
   <si>
     <t>Component LOC</t>
+  </si>
+  <si>
+    <t>GHTorrent_ID</t>
+  </si>
+  <si>
+    <t>db/ Ownership</t>
+  </si>
+  <si>
+    <t>util/ Ownership</t>
+  </si>
+  <si>
+    <t>grid/ Ownership</t>
+  </si>
+  <si>
+    <t>bin/ Ownership</t>
   </si>
 </sst>
 </file>
@@ -672,9 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1258"/>
+  <dimension ref="A1:V1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -691,11 +705,15 @@
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="16" max="17" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -713,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -723,7 +741,7 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
@@ -744,10 +762,25 @@
       <c r="R1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>505949</v>
+      </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="3"/>
@@ -757,7 +790,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2">
         <f>SUM(H3, H4,H6,H7,H8,H9,H10,H11,H11,H12)</f>
@@ -774,7 +807,7 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -782,13 +815,25 @@
       <c r="R2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="3">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -806,7 +851,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3">
         <f>SUM(H5,H13,H21)</f>
@@ -823,7 +868,7 @@
       </c>
       <c r="O3" s="1"/>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -831,13 +876,25 @@
       <c r="R3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3">
         <v>0.92600000000000005</v>
@@ -852,7 +909,7 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4">
         <f>SUM(H16,H20)</f>
@@ -869,7 +926,7 @@
       </c>
       <c r="O4" s="1"/>
       <c r="P4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q4">
         <v>2</v>
@@ -877,10 +934,22 @@
       <c r="R4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3">
         <v>7.2999999999999995E-2</v>
@@ -898,7 +967,7 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5">
         <f>H19</f>
@@ -915,12 +984,12 @@
       </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -930,18 +999,18 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6">
-        <f>E6*F7</f>
+        <f t="shared" ref="H6:H11" si="0">E6*F7</f>
         <v>30</v>
       </c>
       <c r="I6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -951,18 +1020,18 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7">
-        <f>E7*F8</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -972,18 +1041,18 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8">
-        <f>E8*F9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -993,18 +1062,18 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9">
-        <f>E9*F10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1014,18 +1083,18 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10">
-        <f>E10*F11</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="I10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1035,18 +1104,18 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11">
-        <f>E11*F12</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="I11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2">
         <v>0.89200000000000002</v>
@@ -1062,9 +1131,9 @@
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="2">
         <v>0.107</v>
@@ -1077,21 +1146,24 @@
       <c r="I13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="G14" s="3"/>
       <c r="I14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>505901</v>
+      </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15">
@@ -1101,12 +1173,12 @@
       <c r="I15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1125,26 +1197,29 @@
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G17" s="3"/>
       <c r="I17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>505916</v>
+      </c>
       <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="3"/>
       <c r="G18" s="3"/>
       <c r="I18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2">
         <v>0.28000000000000003</v>
@@ -1163,9 +1238,9 @@
       <c r="I19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="2">
         <v>0.17199999999999999</v>
@@ -1184,9 +1259,9 @@
       <c r="I20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="2">
         <v>0.54600000000000004</v>
@@ -1205,56 +1280,56 @@
       <c r="I21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G22" s="3"/>
       <c r="I22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="I24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
       <c r="I25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="I26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
       <c r="I27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="I28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="I29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="I30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="I31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="I32" s="1"/>
       <c r="O32" s="1"/>
@@ -5039,15 +5114,15 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5055,7 +5130,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5063,7 +5138,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -5072,7 +5147,7 @@
         <v>0.92600000000000005</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5080,7 +5155,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5089,13 +5164,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -5103,12 +5178,12 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -5117,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -5125,13 +5200,13 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K21" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N23" s="2"/>
     </row>
@@ -5143,12 +5218,12 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K27" s="2"/>
     </row>
@@ -5160,12 +5235,12 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K31" s="2"/>
       <c r="N31" s="2"/>
@@ -5175,7 +5250,7 @@
         <v>0.89200000000000002</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -5183,31 +5258,31 @@
         <v>0.107</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
         <v>26</v>
-      </c>
-      <c r="C35" t="s">
-        <v>27</v>
       </c>
       <c r="K35" s="2"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K36" s="2"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N38" s="2"/>
     </row>
@@ -5216,21 +5291,21 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K42" s="2"/>
       <c r="N42" s="2"/>
@@ -5240,7 +5315,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -5248,7 +5323,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -5256,7 +5331,7 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2"/>
       <c r="N46" s="2"/>
@@ -5295,21 +5370,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -5317,13 +5392,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -5331,13 +5406,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5345,13 +5420,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>30</v>
@@ -5359,13 +5434,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -5373,13 +5448,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -5387,13 +5462,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -5401,13 +5476,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>-1</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -5415,13 +5490,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -5429,7 +5504,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -5437,7 +5512,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>-1</v>
@@ -5445,13 +5520,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>28</v>
@@ -5459,7 +5534,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -5467,7 +5542,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -5519,10 +5594,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -5530,10 +5605,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5541,18 +5616,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -5560,18 +5635,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -5579,10 +5654,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -5590,18 +5665,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5609,10 +5684,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -5620,10 +5695,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -5631,10 +5706,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>28</v>

</xml_diff>

<commit_message>
Fixed Jan_2008 Data. Fixed Feb_2008 data
</commit_message>
<xml_diff>
--- a/Jan_2008_Sample.xlsx
+++ b/Jan_2008_Sample.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Jan 2008 (Sample)" sheetId="2" r:id="rId1"/>
+    <sheet name="Jan 2008 (Sample)0" sheetId="2" r:id="rId1"/>
     <sheet name="RAW DATA" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Jan_2008_Contributors" localSheetId="0">'Jan 2008 (Sample)'!$B$2:$C$3</definedName>
-    <definedName name="Jan_2008_Contributors_1" localSheetId="0">'Jan 2008 (Sample)'!$B$4:$C$4</definedName>
-    <definedName name="Jan_2008_LOC_1" localSheetId="3">Sheet2!$A$1:$D$12</definedName>
+    <definedName name="Jan_2008_Contributors" localSheetId="0">'Jan 2008 (Sample)0'!$B$2:$C$3</definedName>
+    <definedName name="Jan_2008_Contributors_1" localSheetId="0">'Jan 2008 (Sample)0'!$B$4:$C$4</definedName>
+    <definedName name="Jan_2008_LOC" localSheetId="3">Sheet2!$A$1:$D$12</definedName>
     <definedName name="Jan_2008_test_2" localSheetId="1">'RAW DATA'!$A$1:$C$46</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="46">
   <si>
     <t xml:space="preserve">Contributor Name </t>
   </si>
@@ -406,11 +406,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_Contributors_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_Contributors" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_Contributors" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_Contributors_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_LOC_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_LOC" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,8 +793,8 @@
         <v>15</v>
       </c>
       <c r="K2">
-        <f>SUM(H3, H4,H6,H7,H8,H9,H10,H11,H11,H12)</f>
-        <v>117.902</v>
+        <f>SUMPRODUCT(SUMIF($D$1:$D$21,J2,$H$1:$H$21))</f>
+        <v>105.75399999999999</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="3">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="U2" s="3">
         <v>0</v>
@@ -839,23 +839,23 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3">
-        <f>SUM(H3, H4,H6,H7,H8,H9,H10,H11,H11,H12)/K2</f>
+        <f>SUMPRODUCT(SUMIF($D$1:$D$13,J2,$H$1:$H$21))/K2</f>
         <v>1</v>
       </c>
       <c r="H3">
         <f>E3*F3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
         <v>17</v>
       </c>
       <c r="K3">
-        <f>SUM(H5,H13,H21)</f>
-        <v>8.5289999999999999</v>
+        <f>SUMPRODUCT(SUMIF($D$1:$D$21,J3,$H$1:$H$21))</f>
+        <v>8.6750000000000007</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="U3" s="3">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
       <c r="V3" s="3">
         <v>0</v>
@@ -900,20 +900,20 @@
         <v>0.92600000000000005</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4">
         <f>E4*F4</f>
-        <v>0.92600000000000005</v>
+        <v>2.778</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
         <v>29</v>
       </c>
       <c r="K4">
-        <f>SUM(H16,H20)</f>
-        <v>7.72</v>
+        <f t="shared" ref="K3:K5" si="0">SUMPRODUCT(SUMIF($D$1:$D$21,J4,$H$1:$H$21))</f>
+        <v>9.7199999999999989</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -938,10 +938,10 @@
         <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="U4" s="3">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="V4" s="3">
         <v>1</v>
@@ -955,22 +955,22 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
         <f>SUM(H5,H13)/K3</f>
-        <v>0.35983116426310235</v>
+        <v>0.37060518731988468</v>
       </c>
       <c r="H5">
         <f>E5*F4</f>
-        <v>7.2999999999999995E-2</v>
+        <v>0.21899999999999997</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
         <v>32</v>
       </c>
       <c r="K5">
-        <f>H19</f>
+        <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
       <c r="L5">
@@ -999,8 +999,8 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6">
-        <f t="shared" ref="H6:H11" si="0">E6*F7</f>
-        <v>30</v>
+        <f t="shared" ref="H6:H11" si="1">E6*F7</f>
+        <v>32</v>
       </c>
       <c r="I6" s="1"/>
       <c r="O6" s="1"/>
@@ -1016,12 +1016,12 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="I7" s="1"/>
       <c r="O7" s="1"/>
@@ -1037,11 +1037,11 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="1"/>
@@ -1062,8 +1062,8 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I9" s="1"/>
       <c r="O9" s="1"/>
@@ -1079,12 +1079,12 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I10" s="1"/>
       <c r="O10" s="1"/>
@@ -1100,11 +1100,11 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I11" s="1"/>
@@ -1184,15 +1184,15 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G16" s="3">
         <f>H16/K4</f>
-        <v>0.77720207253886009</v>
+        <v>0.82304526748971207</v>
       </c>
       <c r="H16">
         <f>F16*E16</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="G20" s="3">
         <f>H20/K4</f>
-        <v>0.22279792746113988</v>
+        <v>0.17695473251028807</v>
       </c>
       <c r="H20">
         <f>E20*F20</f>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="G21" s="3">
         <f>SUM(H21)/K3</f>
-        <v>0.64016883573689776</v>
+        <v>0.62939481268011532</v>
       </c>
       <c r="H21">
         <f>E21*F20</f>
@@ -5082,10 +5082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5096,7 +5096,7 @@
     <col min="4" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.85546875" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
@@ -5107,85 +5107,235 @@
     <col min="16" max="16" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" t="str">
+        <f>IFERROR(HLOOKUP(A2,$H4:BG$5,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>IFERROR(HLOOKUP($A2,$H$4:$S$5,2,FALSE),"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D46" si="0">IFERROR(HLOOKUP($A3,$H$4:$S$5,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>32</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>0.92600000000000005</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
@@ -5194,23 +5344,49 @@
       <c r="C19" t="s">
         <v>15</v>
       </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -5220,14 +5396,32 @@
       <c r="C25" t="s">
         <v>15</v>
       </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -5237,13 +5431,33 @@
       <c r="C29" t="s">
         <v>15</v>
       </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="K31" s="2"/>
       <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
@@ -5252,6 +5466,10 @@
       <c r="C33" t="s">
         <v>15</v>
       </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
@@ -5260,6 +5478,10 @@
       <c r="C34" t="s">
         <v>17</v>
       </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -5271,6 +5493,10 @@
       <c r="C35" t="s">
         <v>26</v>
       </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="K35" s="2"/>
       <c r="N35" s="2"/>
     </row>
@@ -5278,13 +5504,33 @@
       <c r="A36" t="s">
         <v>27</v>
       </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
@@ -5293,6 +5539,10 @@
       <c r="C40" t="s">
         <v>29</v>
       </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -5301,14 +5551,28 @@
       <c r="B41" t="s">
         <v>30</v>
       </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="K42" s="2"/>
       <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
@@ -5317,6 +5581,10 @@
       <c r="C44" t="s">
         <v>32</v>
       </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
@@ -5325,6 +5593,10 @@
       <c r="C45" t="s">
         <v>29</v>
       </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
@@ -5332,6 +5604,10 @@
       </c>
       <c r="C46" t="s">
         <v>17</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="K46" s="2"/>
       <c r="N46" s="2"/>
@@ -5558,7 +5834,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C12" sqref="B1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5600,7 +5876,7 @@
         <v>14</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5611,7 +5887,7 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5630,7 +5906,7 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5649,7 +5925,7 @@
         <v>28</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5660,7 +5936,7 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5679,7 +5955,7 @@
         <v>22</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5701,7 +5977,7 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>